<commit_message>
addedheatmaps and dist to shoreline
</commit_message>
<xml_diff>
--- a/data/raw/Aggdata_June52025.xlsx
+++ b/data/raw/Aggdata_June52025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TURNERN\Documents\For Github\Aggregations-Goldfish-HH\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6F809C8-722B-4E0E-9C38-7E4AE1DF8052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C16D415-DAF7-443B-BD9A-131FF75555D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-3285" windowWidth="29040" windowHeight="15720" xr2:uid="{11DCA3BF-F061-428E-80E7-139B1AF39822}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{11DCA3BF-F061-428E-80E7-139B1AF39822}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="28">
   <si>
     <t>Date</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t>Date_1</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -471,18 +474,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5296770-4EFB-446B-B335-2503BA3702EA}">
-  <dimension ref="A1:O114"/>
+  <dimension ref="A1:P114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D102" sqref="D102"/>
+      <selection activeCell="V16" sqref="V16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -514,22 +517,25 @@
         <v>8</v>
       </c>
       <c r="K1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>45756</v>
       </c>
@@ -561,19 +567,23 @@
         <v>3</v>
       </c>
       <c r="K2">
+        <f>SUM(I2+J2)</f>
+        <v>33</v>
+      </c>
+      <c r="L2">
         <v>7.75</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>13.65</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>19.95</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>0.6</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>45756</v>
       </c>
@@ -604,8 +614,9 @@
       <c r="J3">
         <v>0</v>
       </c>
-      <c r="K3" t="s">
-        <v>16</v>
+      <c r="K3">
+        <f>SUM(I3+J3)</f>
+        <v>1</v>
       </c>
       <c r="L3" t="s">
         <v>16</v>
@@ -616,8 +627,11 @@
       <c r="N3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>45756</v>
       </c>
@@ -648,8 +662,9 @@
       <c r="J4">
         <v>0</v>
       </c>
-      <c r="K4" t="s">
-        <v>16</v>
+      <c r="K4">
+        <f t="shared" ref="K4:K67" si="0">SUM(I4+J4)</f>
+        <v>1</v>
       </c>
       <c r="L4" t="s">
         <v>16</v>
@@ -660,8 +675,11 @@
       <c r="N4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>45756</v>
       </c>
@@ -692,8 +710,9 @@
       <c r="J5">
         <v>1</v>
       </c>
-      <c r="K5" t="s">
-        <v>16</v>
+      <c r="K5">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="L5" t="s">
         <v>16</v>
@@ -704,8 +723,11 @@
       <c r="N5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>45756</v>
       </c>
@@ -736,8 +758,9 @@
       <c r="J6">
         <v>0</v>
       </c>
-      <c r="K6" t="s">
-        <v>16</v>
+      <c r="K6">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="L6" t="s">
         <v>16</v>
@@ -748,8 +771,11 @@
       <c r="N6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>45756</v>
       </c>
@@ -780,8 +806,9 @@
       <c r="J7">
         <v>0</v>
       </c>
-      <c r="K7" t="s">
-        <v>16</v>
+      <c r="K7">
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="L7" t="s">
         <v>16</v>
@@ -792,8 +819,11 @@
       <c r="N7" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>45756</v>
       </c>
@@ -824,8 +854,9 @@
       <c r="J8">
         <v>1</v>
       </c>
-      <c r="K8" t="s">
-        <v>16</v>
+      <c r="K8">
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="L8" t="s">
         <v>16</v>
@@ -836,8 +867,11 @@
       <c r="N8" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>45756</v>
       </c>
@@ -868,8 +902,9 @@
       <c r="J9">
         <v>1</v>
       </c>
-      <c r="K9" t="s">
-        <v>16</v>
+      <c r="K9">
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="L9" t="s">
         <v>16</v>
@@ -880,8 +915,11 @@
       <c r="N9" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>45757</v>
       </c>
@@ -912,8 +950,9 @@
       <c r="J10">
         <v>0</v>
       </c>
-      <c r="K10" t="s">
-        <v>16</v>
+      <c r="K10">
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="L10" t="s">
         <v>16</v>
@@ -924,8 +963,11 @@
       <c r="N10" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>45757</v>
       </c>
@@ -956,8 +998,9 @@
       <c r="J11">
         <v>0</v>
       </c>
-      <c r="K11" t="s">
-        <v>16</v>
+      <c r="K11">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="L11" t="s">
         <v>16</v>
@@ -968,8 +1011,11 @@
       <c r="N11" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>45757</v>
       </c>
@@ -1000,8 +1046,9 @@
       <c r="J12">
         <v>0</v>
       </c>
-      <c r="K12" t="s">
-        <v>16</v>
+      <c r="K12">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="L12" t="s">
         <v>16</v>
@@ -1012,8 +1059,11 @@
       <c r="N12" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>45757</v>
       </c>
@@ -1044,8 +1094,9 @@
       <c r="J13">
         <v>0</v>
       </c>
-      <c r="K13" t="s">
-        <v>16</v>
+      <c r="K13">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="L13" t="s">
         <v>16</v>
@@ -1056,8 +1107,11 @@
       <c r="N13" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>45757</v>
       </c>
@@ -1088,8 +1142,9 @@
       <c r="J14">
         <v>1</v>
       </c>
-      <c r="K14" t="s">
-        <v>16</v>
+      <c r="K14">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="L14" t="s">
         <v>16</v>
@@ -1100,8 +1155,11 @@
       <c r="N14" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>45762</v>
       </c>
@@ -1132,8 +1190,9 @@
       <c r="J15">
         <v>0</v>
       </c>
-      <c r="K15" t="s">
-        <v>16</v>
+      <c r="K15">
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="L15" t="s">
         <v>16</v>
@@ -1144,8 +1203,11 @@
       <c r="N15" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>45762</v>
       </c>
@@ -1176,8 +1238,9 @@
       <c r="J16">
         <v>1</v>
       </c>
-      <c r="K16" t="s">
-        <v>16</v>
+      <c r="K16">
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="L16" t="s">
         <v>16</v>
@@ -1188,8 +1251,11 @@
       <c r="N16" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>45762</v>
       </c>
@@ -1220,8 +1286,9 @@
       <c r="J17">
         <v>1</v>
       </c>
-      <c r="K17" t="s">
-        <v>16</v>
+      <c r="K17">
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="L17" t="s">
         <v>16</v>
@@ -1232,8 +1299,11 @@
       <c r="N17" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>45762</v>
       </c>
@@ -1264,8 +1334,9 @@
       <c r="J18">
         <v>3</v>
       </c>
-      <c r="K18" t="s">
-        <v>16</v>
+      <c r="K18">
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
       <c r="L18" t="s">
         <v>16</v>
@@ -1276,8 +1347,11 @@
       <c r="N18" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>45761</v>
       </c>
@@ -1309,19 +1383,23 @@
         <v>1</v>
       </c>
       <c r="K19">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="L19">
         <v>9.3800000000000008</v>
       </c>
-      <c r="L19">
+      <c r="M19">
         <v>11.7</v>
       </c>
-      <c r="M19" t="s">
-        <v>16</v>
-      </c>
       <c r="N19" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>45761</v>
       </c>
@@ -1352,8 +1430,9 @@
       <c r="J20">
         <v>0</v>
       </c>
-      <c r="K20" t="s">
-        <v>16</v>
+      <c r="K20">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="L20" t="s">
         <v>16</v>
@@ -1364,8 +1443,11 @@
       <c r="N20" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>45761</v>
       </c>
@@ -1396,8 +1478,9 @@
       <c r="J21">
         <v>0</v>
       </c>
-      <c r="K21" t="s">
-        <v>16</v>
+      <c r="K21">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="L21" t="s">
         <v>16</v>
@@ -1408,8 +1491,11 @@
       <c r="N21" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O21" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>45761</v>
       </c>
@@ -1440,8 +1526,9 @@
       <c r="J22">
         <v>0</v>
       </c>
-      <c r="K22" t="s">
-        <v>16</v>
+      <c r="K22">
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="L22" t="s">
         <v>16</v>
@@ -1452,8 +1539,11 @@
       <c r="N22" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O22" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>45761</v>
       </c>
@@ -1484,8 +1574,9 @@
       <c r="J23">
         <v>0</v>
       </c>
-      <c r="K23" t="s">
-        <v>16</v>
+      <c r="K23">
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="L23" t="s">
         <v>16</v>
@@ -1496,8 +1587,11 @@
       <c r="N23" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O23" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>45761</v>
       </c>
@@ -1528,8 +1622,9 @@
       <c r="J24">
         <v>1</v>
       </c>
-      <c r="K24" t="s">
-        <v>16</v>
+      <c r="K24">
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="L24" t="s">
         <v>16</v>
@@ -1540,8 +1635,11 @@
       <c r="N24" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>45761</v>
       </c>
@@ -1573,19 +1671,23 @@
         <v>7</v>
       </c>
       <c r="K25">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="L25">
         <v>13.19</v>
       </c>
-      <c r="L25">
+      <c r="M25">
         <v>8.33</v>
       </c>
-      <c r="M25">
+      <c r="N25">
         <v>67.599999999999994</v>
       </c>
-      <c r="N25">
+      <c r="O25">
         <v>0.38</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>45761</v>
       </c>
@@ -1616,8 +1718,9 @@
       <c r="J26">
         <v>1</v>
       </c>
-      <c r="K26" t="s">
-        <v>16</v>
+      <c r="K26">
+        <f t="shared" si="0"/>
+        <v>31</v>
       </c>
       <c r="L26" t="s">
         <v>16</v>
@@ -1628,8 +1731,11 @@
       <c r="N26" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O26" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>45761</v>
       </c>
@@ -1661,19 +1767,23 @@
         <v>4</v>
       </c>
       <c r="K27">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="L27">
         <v>13.14</v>
       </c>
-      <c r="L27">
+      <c r="M27">
         <v>10.57</v>
       </c>
-      <c r="M27">
+      <c r="N27">
         <v>155</v>
       </c>
-      <c r="N27">
+      <c r="O27">
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>45761</v>
       </c>
@@ -1705,19 +1815,23 @@
         <v>0</v>
       </c>
       <c r="K28">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="L28">
         <v>12.69</v>
       </c>
-      <c r="L28">
+      <c r="M28">
         <v>10.99</v>
       </c>
-      <c r="M28">
+      <c r="N28">
         <v>48.8</v>
       </c>
-      <c r="N28">
+      <c r="O28">
         <v>0.45</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>45761</v>
       </c>
@@ -1748,8 +1862,9 @@
       <c r="J29">
         <v>0</v>
       </c>
-      <c r="K29" t="s">
-        <v>16</v>
+      <c r="K29">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="L29" t="s">
         <v>16</v>
@@ -1760,8 +1875,11 @@
       <c r="N29" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O29" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>45761</v>
       </c>
@@ -1792,8 +1910,9 @@
       <c r="J30">
         <v>0</v>
       </c>
-      <c r="K30" t="s">
-        <v>16</v>
+      <c r="K30">
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="L30" t="s">
         <v>16</v>
@@ -1804,8 +1923,11 @@
       <c r="N30" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O30" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>45761</v>
       </c>
@@ -1836,8 +1958,9 @@
       <c r="J31">
         <v>0</v>
       </c>
-      <c r="K31" t="s">
-        <v>16</v>
+      <c r="K31">
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
       <c r="L31" t="s">
         <v>16</v>
@@ -1848,8 +1971,11 @@
       <c r="N31" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O31" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>45761</v>
       </c>
@@ -1880,8 +2006,9 @@
       <c r="J32">
         <v>0</v>
       </c>
-      <c r="K32" t="s">
-        <v>16</v>
+      <c r="K32">
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="L32" t="s">
         <v>16</v>
@@ -1892,8 +2019,11 @@
       <c r="N32" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O32" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>45761</v>
       </c>
@@ -1924,8 +2054,9 @@
       <c r="J33">
         <v>0</v>
       </c>
-      <c r="K33" t="s">
-        <v>16</v>
+      <c r="K33">
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="L33" t="s">
         <v>16</v>
@@ -1936,8 +2067,11 @@
       <c r="N33" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O33" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>45761</v>
       </c>
@@ -1968,8 +2102,9 @@
       <c r="J34">
         <v>0</v>
       </c>
-      <c r="K34" t="s">
-        <v>16</v>
+      <c r="K34">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="L34" t="s">
         <v>16</v>
@@ -1980,8 +2115,11 @@
       <c r="N34" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O34" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>45761</v>
       </c>
@@ -2012,8 +2150,9 @@
       <c r="J35">
         <v>1</v>
       </c>
-      <c r="K35" t="s">
-        <v>16</v>
+      <c r="K35">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="L35" t="s">
         <v>16</v>
@@ -2024,8 +2163,11 @@
       <c r="N35" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O35" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>45761</v>
       </c>
@@ -2057,19 +2199,23 @@
         <v>0</v>
       </c>
       <c r="K36">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="L36">
         <v>13.08</v>
       </c>
-      <c r="L36">
+      <c r="M36">
         <v>9.9700000000000006</v>
       </c>
-      <c r="M36">
+      <c r="N36">
         <v>37.049999999999997</v>
       </c>
-      <c r="N36">
+      <c r="O36">
         <v>0.52</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>45761</v>
       </c>
@@ -2101,19 +2247,23 @@
         <v>4</v>
       </c>
       <c r="K37">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="L37">
         <v>13.78</v>
       </c>
-      <c r="L37">
+      <c r="M37">
         <v>9.8699999999999992</v>
       </c>
-      <c r="M37">
+      <c r="N37">
         <v>47</v>
       </c>
-      <c r="N37">
+      <c r="O37">
         <v>0.7</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>45761</v>
       </c>
@@ -2144,8 +2294,9 @@
       <c r="J38">
         <v>2</v>
       </c>
-      <c r="K38" t="s">
-        <v>16</v>
+      <c r="K38">
+        <f t="shared" si="0"/>
+        <v>32</v>
       </c>
       <c r="L38" t="s">
         <v>16</v>
@@ -2156,8 +2307,11 @@
       <c r="N38" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O38" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>45761</v>
       </c>
@@ -2189,19 +2343,23 @@
         <v>8</v>
       </c>
       <c r="K39">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="L39">
         <v>13.45</v>
       </c>
-      <c r="L39">
+      <c r="M39">
         <v>12.74</v>
       </c>
-      <c r="M39">
+      <c r="N39">
         <v>47</v>
       </c>
-      <c r="N39">
+      <c r="O39">
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>45761</v>
       </c>
@@ -2234,22 +2392,26 @@
         <v>8</v>
       </c>
       <c r="K40">
+        <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
+      <c r="L40">
         <v>13.01</v>
       </c>
-      <c r="L40">
+      <c r="M40">
         <v>13.3</v>
       </c>
-      <c r="M40">
+      <c r="N40">
         <v>46</v>
       </c>
-      <c r="N40">
+      <c r="O40">
         <v>0.48</v>
       </c>
-      <c r="O40" t="s">
+      <c r="P40" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>45761</v>
       </c>
@@ -2280,8 +2442,9 @@
       <c r="J41">
         <v>12</v>
       </c>
-      <c r="K41" t="s">
-        <v>16</v>
+      <c r="K41">
+        <f t="shared" si="0"/>
+        <v>30</v>
       </c>
       <c r="L41" t="s">
         <v>16</v>
@@ -2292,8 +2455,11 @@
       <c r="N41" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O41" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>45761</v>
       </c>
@@ -2324,8 +2490,9 @@
       <c r="J42">
         <v>0</v>
       </c>
-      <c r="K42" t="s">
-        <v>16</v>
+      <c r="K42">
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="L42" t="s">
         <v>16</v>
@@ -2336,8 +2503,11 @@
       <c r="N42" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O42" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>45761</v>
       </c>
@@ -2368,8 +2538,9 @@
       <c r="J43">
         <v>0</v>
       </c>
-      <c r="K43" t="s">
-        <v>16</v>
+      <c r="K43">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="L43" t="s">
         <v>16</v>
@@ -2380,8 +2551,11 @@
       <c r="N43" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O43" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>45761</v>
       </c>
@@ -2412,8 +2586,9 @@
       <c r="J44">
         <v>0</v>
       </c>
-      <c r="K44" t="s">
-        <v>16</v>
+      <c r="K44">
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="L44" t="s">
         <v>16</v>
@@ -2424,8 +2599,11 @@
       <c r="N44" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O44" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>45769</v>
       </c>
@@ -2456,8 +2634,9 @@
       <c r="J45">
         <v>1</v>
       </c>
-      <c r="K45" t="s">
-        <v>16</v>
+      <c r="K45">
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="L45" t="s">
         <v>16</v>
@@ -2468,8 +2647,11 @@
       <c r="N45" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O45" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>45769</v>
       </c>
@@ -2500,8 +2682,9 @@
       <c r="J46">
         <v>1</v>
       </c>
-      <c r="K46" t="s">
-        <v>16</v>
+      <c r="K46">
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
       <c r="L46" t="s">
         <v>16</v>
@@ -2512,8 +2695,11 @@
       <c r="N46" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O46" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>45769</v>
       </c>
@@ -2544,8 +2730,9 @@
       <c r="J47">
         <v>0</v>
       </c>
-      <c r="K47" t="s">
-        <v>16</v>
+      <c r="K47">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="L47" t="s">
         <v>16</v>
@@ -2556,8 +2743,11 @@
       <c r="N47" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O47" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>45769</v>
       </c>
@@ -2589,19 +2779,23 @@
         <v>2</v>
       </c>
       <c r="K48">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="L48">
         <v>10.44</v>
       </c>
-      <c r="L48">
+      <c r="M48">
         <v>11.27</v>
       </c>
-      <c r="M48">
+      <c r="N48">
         <v>13.16</v>
       </c>
-      <c r="N48">
+      <c r="O48">
         <v>0.63</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>45769</v>
       </c>
@@ -2632,8 +2826,9 @@
       <c r="J49">
         <v>2</v>
       </c>
-      <c r="K49" t="s">
-        <v>16</v>
+      <c r="K49">
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="L49" t="s">
         <v>16</v>
@@ -2644,8 +2839,11 @@
       <c r="N49" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O49" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>45769</v>
       </c>
@@ -2676,8 +2874,9 @@
       <c r="J50">
         <v>0</v>
       </c>
-      <c r="K50" t="s">
-        <v>16</v>
+      <c r="K50">
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="L50" t="s">
         <v>16</v>
@@ -2688,8 +2887,11 @@
       <c r="N50" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O50" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>45769</v>
       </c>
@@ -2721,19 +2923,23 @@
         <v>0</v>
       </c>
       <c r="K51">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="L51">
         <v>10.92</v>
       </c>
-      <c r="L51">
+      <c r="M51">
         <v>11.24</v>
       </c>
-      <c r="M51">
+      <c r="N51">
         <v>14.5</v>
       </c>
-      <c r="N51">
+      <c r="O51">
         <v>0.7</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>45769</v>
       </c>
@@ -2764,8 +2970,9 @@
       <c r="J52">
         <v>1</v>
       </c>
-      <c r="K52" t="s">
-        <v>16</v>
+      <c r="K52">
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="L52" t="s">
         <v>16</v>
@@ -2776,8 +2983,11 @@
       <c r="N52" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O52" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>45769</v>
       </c>
@@ -2808,8 +3018,9 @@
       <c r="J53">
         <v>0</v>
       </c>
-      <c r="K53" t="s">
-        <v>16</v>
+      <c r="K53">
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="L53" t="s">
         <v>16</v>
@@ -2820,8 +3031,11 @@
       <c r="N53" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O53" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>45769</v>
       </c>
@@ -2852,8 +3066,9 @@
       <c r="J54">
         <v>0</v>
       </c>
-      <c r="K54" t="s">
-        <v>16</v>
+      <c r="K54">
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="L54" t="s">
         <v>16</v>
@@ -2864,8 +3079,11 @@
       <c r="N54" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O54" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>45769</v>
       </c>
@@ -2896,8 +3114,9 @@
       <c r="J55">
         <v>0</v>
       </c>
-      <c r="K55" t="s">
-        <v>16</v>
+      <c r="K55">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="L55" t="s">
         <v>16</v>
@@ -2908,8 +3127,11 @@
       <c r="N55" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O55" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>45769</v>
       </c>
@@ -2940,8 +3162,9 @@
       <c r="J56">
         <v>0</v>
       </c>
-      <c r="K56" t="s">
-        <v>16</v>
+      <c r="K56">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="L56" t="s">
         <v>16</v>
@@ -2952,8 +3175,11 @@
       <c r="N56" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O56" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>45769</v>
       </c>
@@ -2984,8 +3210,9 @@
       <c r="J57">
         <v>0</v>
       </c>
-      <c r="K57" t="s">
-        <v>16</v>
+      <c r="K57">
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="L57" t="s">
         <v>16</v>
@@ -2996,8 +3223,11 @@
       <c r="N57" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O57" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>45769</v>
       </c>
@@ -3029,16 +3259,20 @@
         <v>3</v>
       </c>
       <c r="K58">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="L58">
         <v>13.66</v>
       </c>
-      <c r="L58">
+      <c r="M58">
         <v>11.01</v>
       </c>
-      <c r="N58">
+      <c r="O58">
         <v>0.68</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>45769</v>
       </c>
@@ -3070,22 +3304,26 @@
         <v>20</v>
       </c>
       <c r="K59">
+        <f t="shared" si="0"/>
+        <v>77</v>
+      </c>
+      <c r="L59">
         <v>15.39</v>
       </c>
-      <c r="L59">
+      <c r="M59">
         <v>8.7200000000000006</v>
       </c>
-      <c r="M59">
+      <c r="N59">
         <v>174</v>
       </c>
-      <c r="N59">
+      <c r="O59">
         <v>0.5</v>
       </c>
-      <c r="O59" t="s">
+      <c r="P59" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>45769</v>
       </c>
@@ -3116,8 +3354,9 @@
       <c r="J60">
         <v>0</v>
       </c>
-      <c r="K60" t="s">
-        <v>16</v>
+      <c r="K60">
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="L60" t="s">
         <v>16</v>
@@ -3129,10 +3368,13 @@
         <v>16</v>
       </c>
       <c r="O60" t="s">
+        <v>16</v>
+      </c>
+      <c r="P60" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>45769</v>
       </c>
@@ -3163,8 +3405,9 @@
       <c r="J61">
         <v>0</v>
       </c>
-      <c r="K61" t="s">
-        <v>16</v>
+      <c r="K61">
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
       <c r="L61" t="s">
         <v>16</v>
@@ -3176,10 +3419,13 @@
         <v>16</v>
       </c>
       <c r="O61" t="s">
+        <v>16</v>
+      </c>
+      <c r="P61" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>45769</v>
       </c>
@@ -3210,8 +3456,9 @@
       <c r="J62">
         <v>0</v>
       </c>
-      <c r="K62" t="s">
-        <v>16</v>
+      <c r="K62">
+        <f t="shared" si="0"/>
+        <v>17</v>
       </c>
       <c r="L62" t="s">
         <v>16</v>
@@ -3223,10 +3470,13 @@
         <v>16</v>
       </c>
       <c r="O62" t="s">
+        <v>16</v>
+      </c>
+      <c r="P62" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>45769</v>
       </c>
@@ -3258,19 +3508,23 @@
         <v>4</v>
       </c>
       <c r="K63">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="L63">
         <v>15.52</v>
       </c>
-      <c r="L63">
+      <c r="M63">
         <v>9.93</v>
       </c>
-      <c r="M63">
+      <c r="N63">
         <v>65.83</v>
       </c>
-      <c r="N63">
+      <c r="O63">
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>45769</v>
       </c>
@@ -3301,8 +3555,9 @@
       <c r="J64">
         <v>1</v>
       </c>
-      <c r="K64" t="s">
-        <v>16</v>
+      <c r="K64">
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="L64" t="s">
         <v>16</v>
@@ -3313,8 +3568,11 @@
       <c r="N64" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O64" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>45769</v>
       </c>
@@ -3345,8 +3603,9 @@
       <c r="J65">
         <v>1</v>
       </c>
-      <c r="K65" t="s">
-        <v>16</v>
+      <c r="K65">
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="L65" t="s">
         <v>16</v>
@@ -3357,8 +3616,11 @@
       <c r="N65" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O65" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>45769</v>
       </c>
@@ -3389,8 +3651,9 @@
       <c r="J66">
         <v>3</v>
       </c>
-      <c r="K66" t="s">
-        <v>16</v>
+      <c r="K66">
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="L66" t="s">
         <v>16</v>
@@ -3401,8 +3664,11 @@
       <c r="N66" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O66" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>45769</v>
       </c>
@@ -3434,19 +3700,23 @@
         <v>2</v>
       </c>
       <c r="K67">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="L67">
         <v>11.9</v>
       </c>
-      <c r="L67">
+      <c r="M67">
         <v>10.18</v>
       </c>
-      <c r="M67">
+      <c r="N67">
         <v>55.65</v>
       </c>
-      <c r="N67">
+      <c r="O67">
         <v>0.75</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>45770</v>
       </c>
@@ -3477,8 +3747,9 @@
       <c r="J68">
         <v>1</v>
       </c>
-      <c r="K68" t="s">
-        <v>16</v>
+      <c r="K68">
+        <f t="shared" ref="K68:K114" si="1">SUM(I68+J68)</f>
+        <v>1</v>
       </c>
       <c r="L68" t="s">
         <v>16</v>
@@ -3489,8 +3760,11 @@
       <c r="N68" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O68" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>45770</v>
       </c>
@@ -3521,8 +3795,9 @@
       <c r="J69">
         <v>0</v>
       </c>
-      <c r="K69" t="s">
-        <v>16</v>
+      <c r="K69">
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="L69" t="s">
         <v>16</v>
@@ -3533,8 +3808,11 @@
       <c r="N69" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O69" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>45770</v>
       </c>
@@ -3565,8 +3843,9 @@
       <c r="J70">
         <v>2</v>
       </c>
-      <c r="K70" t="s">
-        <v>16</v>
+      <c r="K70">
+        <f t="shared" si="1"/>
+        <v>3</v>
       </c>
       <c r="L70" t="s">
         <v>16</v>
@@ -3577,8 +3856,11 @@
       <c r="N70" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O70" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>45770</v>
       </c>
@@ -3609,8 +3891,9 @@
       <c r="J71">
         <v>0</v>
       </c>
-      <c r="K71" t="s">
-        <v>16</v>
+      <c r="K71">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="L71" t="s">
         <v>16</v>
@@ -3621,8 +3904,11 @@
       <c r="N71" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O71" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>45775</v>
       </c>
@@ -3653,8 +3939,9 @@
       <c r="J72">
         <v>0</v>
       </c>
-      <c r="K72" t="s">
-        <v>16</v>
+      <c r="K72">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="L72" t="s">
         <v>16</v>
@@ -3665,8 +3952,11 @@
       <c r="N72" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O72" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>45775</v>
       </c>
@@ -3697,8 +3987,9 @@
       <c r="J73">
         <v>0</v>
       </c>
-      <c r="K73" t="s">
-        <v>16</v>
+      <c r="K73">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="L73" t="s">
         <v>16</v>
@@ -3709,8 +4000,11 @@
       <c r="N73" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O73" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>45775</v>
       </c>
@@ -3741,8 +4035,9 @@
       <c r="J74">
         <v>0</v>
       </c>
-      <c r="K74" t="s">
-        <v>16</v>
+      <c r="K74">
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="L74" t="s">
         <v>16</v>
@@ -3753,8 +4048,11 @@
       <c r="N74" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O74" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>45775</v>
       </c>
@@ -3785,8 +4083,9 @@
       <c r="J75">
         <v>0</v>
       </c>
-      <c r="K75" t="s">
-        <v>16</v>
+      <c r="K75">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="L75" t="s">
         <v>16</v>
@@ -3797,8 +4096,11 @@
       <c r="N75" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O75" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>45775</v>
       </c>
@@ -3829,8 +4131,9 @@
       <c r="J76">
         <v>0</v>
       </c>
-      <c r="K76" t="s">
-        <v>16</v>
+      <c r="K76">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="L76" t="s">
         <v>16</v>
@@ -3841,8 +4144,11 @@
       <c r="N76" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O76" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>45775</v>
       </c>
@@ -3873,8 +4179,9 @@
       <c r="J77">
         <v>0</v>
       </c>
-      <c r="K77" t="s">
-        <v>16</v>
+      <c r="K77">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="L77" t="s">
         <v>16</v>
@@ -3885,8 +4192,11 @@
       <c r="N77" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O77" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>45775</v>
       </c>
@@ -3917,8 +4227,9 @@
       <c r="J78">
         <v>0</v>
       </c>
-      <c r="K78" t="s">
-        <v>16</v>
+      <c r="K78">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="L78" t="s">
         <v>16</v>
@@ -3929,8 +4240,11 @@
       <c r="N78" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O78" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>45775</v>
       </c>
@@ -3961,8 +4275,9 @@
       <c r="J79">
         <v>0</v>
       </c>
-      <c r="K79" t="s">
-        <v>16</v>
+      <c r="K79">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="L79" t="s">
         <v>16</v>
@@ -3973,8 +4288,11 @@
       <c r="N79" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O79" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>45775</v>
       </c>
@@ -4006,22 +4324,26 @@
         <v>3</v>
       </c>
       <c r="K80">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="L80">
         <v>16.54</v>
       </c>
-      <c r="L80">
+      <c r="M80">
         <v>11.52</v>
       </c>
-      <c r="M80">
+      <c r="N80">
         <v>13.38</v>
       </c>
-      <c r="N80" t="s">
-        <v>16</v>
-      </c>
       <c r="O80" t="s">
+        <v>16</v>
+      </c>
+      <c r="P80" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>45775</v>
       </c>
@@ -4052,8 +4374,9 @@
       <c r="J81">
         <v>1</v>
       </c>
-      <c r="K81" t="s">
-        <v>16</v>
+      <c r="K81">
+        <f t="shared" si="1"/>
+        <v>6</v>
       </c>
       <c r="L81" t="s">
         <v>16</v>
@@ -4064,8 +4387,11 @@
       <c r="N81" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O81" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>45775</v>
       </c>
@@ -4096,8 +4422,9 @@
       <c r="J82">
         <v>8</v>
       </c>
-      <c r="K82" t="s">
-        <v>16</v>
+      <c r="K82">
+        <f t="shared" si="1"/>
+        <v>11</v>
       </c>
       <c r="L82" t="s">
         <v>16</v>
@@ -4108,8 +4435,11 @@
       <c r="N82" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O82" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>45775</v>
       </c>
@@ -4140,8 +4470,9 @@
       <c r="J83">
         <v>2</v>
       </c>
-      <c r="K83" t="s">
-        <v>16</v>
+      <c r="K83">
+        <f t="shared" si="1"/>
+        <v>5</v>
       </c>
       <c r="L83" t="s">
         <v>16</v>
@@ -4152,8 +4483,11 @@
       <c r="N83" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O83" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>45775</v>
       </c>
@@ -4185,19 +4519,23 @@
         <v>8</v>
       </c>
       <c r="K84">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="L84">
         <v>20</v>
       </c>
-      <c r="L84">
+      <c r="M84">
         <v>8.89</v>
       </c>
-      <c r="M84" t="s">
-        <v>16</v>
-      </c>
-      <c r="N84">
+      <c r="N84" t="s">
+        <v>16</v>
+      </c>
+      <c r="O84">
         <v>0.5</v>
       </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>45775</v>
       </c>
@@ -4228,8 +4566,9 @@
       <c r="J85">
         <v>3</v>
       </c>
-      <c r="K85" t="s">
-        <v>16</v>
+      <c r="K85">
+        <f t="shared" si="1"/>
+        <v>12</v>
       </c>
       <c r="L85" t="s">
         <v>16</v>
@@ -4240,8 +4579,11 @@
       <c r="N85" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O85" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>45775</v>
       </c>
@@ -4272,8 +4614,9 @@
       <c r="J86">
         <v>3</v>
       </c>
-      <c r="K86" t="s">
-        <v>16</v>
+      <c r="K86">
+        <f t="shared" si="1"/>
+        <v>6</v>
       </c>
       <c r="L86" t="s">
         <v>16</v>
@@ -4284,8 +4627,11 @@
       <c r="N86" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O86" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>45775</v>
       </c>
@@ -4316,8 +4662,9 @@
       <c r="J87">
         <v>0</v>
       </c>
-      <c r="K87" t="s">
-        <v>16</v>
+      <c r="K87">
+        <f t="shared" si="1"/>
+        <v>10</v>
       </c>
       <c r="L87" t="s">
         <v>16</v>
@@ -4328,8 +4675,11 @@
       <c r="N87" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O87" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>45775</v>
       </c>
@@ -4360,8 +4710,9 @@
       <c r="J88">
         <v>0</v>
       </c>
-      <c r="K88" t="s">
-        <v>16</v>
+      <c r="K88">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="L88" t="s">
         <v>16</v>
@@ -4372,8 +4723,11 @@
       <c r="N88" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O88" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>45775</v>
       </c>
@@ -4404,8 +4758,9 @@
       <c r="J89">
         <v>0</v>
       </c>
-      <c r="K89" t="s">
-        <v>16</v>
+      <c r="K89">
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="L89" t="s">
         <v>16</v>
@@ -4416,8 +4771,11 @@
       <c r="N89" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O89" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>45775</v>
       </c>
@@ -4448,8 +4806,9 @@
       <c r="J90">
         <v>0</v>
       </c>
-      <c r="K90" t="s">
-        <v>16</v>
+      <c r="K90">
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="L90" t="s">
         <v>16</v>
@@ -4460,8 +4819,11 @@
       <c r="N90" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O90" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>45775</v>
       </c>
@@ -4492,8 +4854,9 @@
       <c r="J91">
         <v>0</v>
       </c>
-      <c r="K91" t="s">
-        <v>16</v>
+      <c r="K91">
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="L91" t="s">
         <v>16</v>
@@ -4504,8 +4867,11 @@
       <c r="N91" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O91" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>45775</v>
       </c>
@@ -4536,8 +4902,9 @@
       <c r="J92">
         <v>0</v>
       </c>
-      <c r="K92" t="s">
-        <v>16</v>
+      <c r="K92">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="L92" t="s">
         <v>16</v>
@@ -4548,8 +4915,11 @@
       <c r="N92" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O92" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>45775</v>
       </c>
@@ -4580,8 +4950,9 @@
       <c r="J93">
         <v>1</v>
       </c>
-      <c r="K93" t="s">
-        <v>16</v>
+      <c r="K93">
+        <f t="shared" si="1"/>
+        <v>3</v>
       </c>
       <c r="L93" t="s">
         <v>16</v>
@@ -4592,8 +4963,11 @@
       <c r="N93" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O93" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>45775</v>
       </c>
@@ -4624,8 +4998,9 @@
       <c r="J94">
         <v>0</v>
       </c>
-      <c r="K94" t="s">
-        <v>16</v>
+      <c r="K94">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="L94" t="s">
         <v>16</v>
@@ -4636,8 +5011,11 @@
       <c r="N94" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O94" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>45775</v>
       </c>
@@ -4668,8 +5046,9 @@
       <c r="J95">
         <v>0</v>
       </c>
-      <c r="K95" t="s">
-        <v>16</v>
+      <c r="K95">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="L95" t="s">
         <v>16</v>
@@ -4680,8 +5059,11 @@
       <c r="N95" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O95" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>45775</v>
       </c>
@@ -4712,8 +5094,9 @@
       <c r="J96">
         <v>0</v>
       </c>
-      <c r="K96" t="s">
-        <v>16</v>
+      <c r="K96">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="L96" t="s">
         <v>16</v>
@@ -4724,8 +5107,11 @@
       <c r="N96" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O96" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>45775</v>
       </c>
@@ -4756,8 +5142,9 @@
       <c r="J97">
         <v>0</v>
       </c>
-      <c r="K97" t="s">
-        <v>16</v>
+      <c r="K97">
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="L97" t="s">
         <v>16</v>
@@ -4768,8 +5155,11 @@
       <c r="N97" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O97" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>45775</v>
       </c>
@@ -4800,8 +5190,9 @@
       <c r="J98">
         <v>0</v>
       </c>
-      <c r="K98" t="s">
-        <v>16</v>
+      <c r="K98">
+        <f t="shared" si="1"/>
+        <v>3</v>
       </c>
       <c r="L98" t="s">
         <v>16</v>
@@ -4812,8 +5203,11 @@
       <c r="N98" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O98" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>45775</v>
       </c>
@@ -4844,8 +5238,9 @@
       <c r="J99">
         <v>0</v>
       </c>
-      <c r="K99" t="s">
-        <v>16</v>
+      <c r="K99">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="L99" t="s">
         <v>16</v>
@@ -4856,8 +5251,11 @@
       <c r="N99" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O99" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>45775</v>
       </c>
@@ -4888,8 +5286,9 @@
       <c r="J100">
         <v>0</v>
       </c>
-      <c r="K100" t="s">
-        <v>16</v>
+      <c r="K100">
+        <f t="shared" si="1"/>
+        <v>3</v>
       </c>
       <c r="L100" t="s">
         <v>16</v>
@@ -4900,8 +5299,11 @@
       <c r="N100" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O100" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>45775</v>
       </c>
@@ -4932,8 +5334,9 @@
       <c r="J101">
         <v>0</v>
       </c>
-      <c r="K101" t="s">
-        <v>16</v>
+      <c r="K101">
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="L101" t="s">
         <v>16</v>
@@ -4944,8 +5347,11 @@
       <c r="N101" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O101" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>45775</v>
       </c>
@@ -4977,22 +5383,26 @@
         <v>10</v>
       </c>
       <c r="K102">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="L102">
         <v>16.989999999999998</v>
       </c>
-      <c r="L102">
+      <c r="M102">
         <v>10.47</v>
       </c>
-      <c r="M102">
+      <c r="N102">
         <v>68</v>
       </c>
-      <c r="N102">
+      <c r="O102">
         <v>0.65</v>
       </c>
-      <c r="O102" t="s">
+      <c r="P102" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>45775</v>
       </c>
@@ -5023,8 +5433,9 @@
       <c r="J103">
         <v>0</v>
       </c>
-      <c r="K103" t="s">
-        <v>16</v>
+      <c r="K103">
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="L103" t="s">
         <v>16</v>
@@ -5035,8 +5446,11 @@
       <c r="N103" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O103" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="104" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>45775</v>
       </c>
@@ -5067,8 +5481,9 @@
       <c r="J104">
         <v>0</v>
       </c>
-      <c r="K104" t="s">
-        <v>16</v>
+      <c r="K104">
+        <f t="shared" si="1"/>
+        <v>5</v>
       </c>
       <c r="L104" t="s">
         <v>16</v>
@@ -5079,8 +5494,11 @@
       <c r="N104" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O104" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>45775</v>
       </c>
@@ -5111,8 +5529,9 @@
       <c r="J105">
         <v>0</v>
       </c>
-      <c r="K105" t="s">
-        <v>16</v>
+      <c r="K105">
+        <f t="shared" si="1"/>
+        <v>5</v>
       </c>
       <c r="L105" t="s">
         <v>16</v>
@@ -5123,8 +5542,11 @@
       <c r="N105" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O105" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>45775</v>
       </c>
@@ -5155,8 +5577,9 @@
       <c r="J106">
         <v>0</v>
       </c>
-      <c r="K106" t="s">
-        <v>16</v>
+      <c r="K106">
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="L106" t="s">
         <v>16</v>
@@ -5167,8 +5590,11 @@
       <c r="N106" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O106" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>45775</v>
       </c>
@@ -5199,8 +5625,9 @@
       <c r="J107">
         <v>0</v>
       </c>
-      <c r="K107" t="s">
-        <v>16</v>
+      <c r="K107">
+        <f t="shared" si="1"/>
+        <v>5</v>
       </c>
       <c r="L107" t="s">
         <v>16</v>
@@ -5211,8 +5638,11 @@
       <c r="N107" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O107" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>45775</v>
       </c>
@@ -5243,8 +5673,9 @@
       <c r="J108">
         <v>0</v>
       </c>
-      <c r="K108" t="s">
-        <v>16</v>
+      <c r="K108">
+        <f t="shared" si="1"/>
+        <v>3</v>
       </c>
       <c r="L108" t="s">
         <v>16</v>
@@ -5255,8 +5686,11 @@
       <c r="N108" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O108" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="109" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>45775</v>
       </c>
@@ -5287,8 +5721,9 @@
       <c r="J109">
         <v>0</v>
       </c>
-      <c r="K109" t="s">
-        <v>16</v>
+      <c r="K109">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="L109" t="s">
         <v>16</v>
@@ -5299,8 +5734,11 @@
       <c r="N109" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O109" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>45775</v>
       </c>
@@ -5331,8 +5769,9 @@
       <c r="J110">
         <v>1</v>
       </c>
-      <c r="K110" t="s">
-        <v>16</v>
+      <c r="K110">
+        <f t="shared" si="1"/>
+        <v>3</v>
       </c>
       <c r="L110" t="s">
         <v>16</v>
@@ -5343,8 +5782,11 @@
       <c r="N110" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O110" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>45775</v>
       </c>
@@ -5375,8 +5817,9 @@
       <c r="J111">
         <v>0</v>
       </c>
-      <c r="K111" t="s">
-        <v>16</v>
+      <c r="K111">
+        <f t="shared" si="1"/>
+        <v>4</v>
       </c>
       <c r="L111" t="s">
         <v>16</v>
@@ -5387,8 +5830,11 @@
       <c r="N111" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O111" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="112" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>45775</v>
       </c>
@@ -5419,8 +5865,9 @@
       <c r="J112">
         <v>0</v>
       </c>
-      <c r="K112" t="s">
-        <v>16</v>
+      <c r="K112">
+        <f t="shared" si="1"/>
+        <v>3</v>
       </c>
       <c r="L112" t="s">
         <v>16</v>
@@ -5431,8 +5878,11 @@
       <c r="N112" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="113" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O112" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="113" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>45775</v>
       </c>
@@ -5463,8 +5913,9 @@
       <c r="J113">
         <v>0</v>
       </c>
-      <c r="K113" t="s">
-        <v>16</v>
+      <c r="K113">
+        <f t="shared" si="1"/>
+        <v>3</v>
       </c>
       <c r="L113" t="s">
         <v>16</v>
@@ -5475,8 +5926,11 @@
       <c r="N113" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="114" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O113" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="114" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>45775</v>
       </c>
@@ -5507,8 +5961,9 @@
       <c r="J114">
         <v>0</v>
       </c>
-      <c r="K114" t="s">
-        <v>16</v>
+      <c r="K114">
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="L114" t="s">
         <v>16</v>
@@ -5517,6 +5972,9 @@
         <v>16</v>
       </c>
       <c r="N114" t="s">
+        <v>16</v>
+      </c>
+      <c r="O114" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>